<commit_message>
Optimization in Joint Space working
</commit_message>
<xml_diff>
--- a/multiuser_legible_movement/data/eval/simulation_results_a.xlsx
+++ b/multiuser_legible_movement/data/eval/simulation_results_a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\My_documents\Instituto.Superior.Tecnico\PhD\movement_communication\multiuser_legible_movement\data\eval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\My_Documents\Instituto.Superior.Tecnico\PhD\movement_communication\multiuser_legible_movement\data\eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1EB4F1-8230-40D9-BC24-212D346E0425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B27969-100A-4388-BFB0-C1A8958A2CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>